<commit_message>
Respetar 5 Lineas por personaje
</commit_message>
<xml_diff>
--- a/prop_optimizada.xlsx
+++ b/prop_optimizada.xlsx
@@ -2455,7 +2455,7 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B23" t="s">
         <v>27</v>
@@ -2478,7 +2478,7 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B24" t="s">
         <v>28</v>
@@ -2501,7 +2501,7 @@
     </row>
     <row r="25" spans="1:7">
       <c r="A25">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B25" t="s">
         <v>29</v>
@@ -2524,7 +2524,7 @@
     </row>
     <row r="26" spans="1:7">
       <c r="A26">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B26" t="s">
         <v>29</v>
@@ -2547,7 +2547,7 @@
     </row>
     <row r="27" spans="1:7">
       <c r="A27">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B27" t="s">
         <v>30</v>
@@ -2570,7 +2570,7 @@
     </row>
     <row r="28" spans="1:7">
       <c r="A28">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B28" t="s">
         <v>30</v>
@@ -2593,7 +2593,7 @@
     </row>
     <row r="29" spans="1:7">
       <c r="A29">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B29" t="s">
         <v>31</v>
@@ -2616,7 +2616,7 @@
     </row>
     <row r="30" spans="1:7">
       <c r="A30">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B30" t="s">
         <v>31</v>
@@ -2639,7 +2639,7 @@
     </row>
     <row r="31" spans="1:7">
       <c r="A31">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B31" t="s">
         <v>31</v>
@@ -2662,7 +2662,7 @@
     </row>
     <row r="32" spans="1:7">
       <c r="A32">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B32" t="s">
         <v>32</v>
@@ -2685,7 +2685,7 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B33" t="s">
         <v>32</v>
@@ -2708,7 +2708,7 @@
     </row>
     <row r="34" spans="1:7">
       <c r="A34">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B34" t="s">
         <v>33</v>
@@ -2731,7 +2731,7 @@
     </row>
     <row r="35" spans="1:7">
       <c r="A35">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B35" t="s">
         <v>34</v>
@@ -2754,7 +2754,7 @@
     </row>
     <row r="36" spans="1:7">
       <c r="A36">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B36" t="s">
         <v>35</v>
@@ -2777,7 +2777,7 @@
     </row>
     <row r="37" spans="1:7">
       <c r="A37">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B37" t="s">
         <v>36</v>
@@ -2800,7 +2800,7 @@
     </row>
     <row r="38" spans="1:7">
       <c r="A38">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B38" t="s">
         <v>36</v>
@@ -2823,7 +2823,7 @@
     </row>
     <row r="39" spans="1:7">
       <c r="A39">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B39" t="s">
         <v>37</v>
@@ -2846,7 +2846,7 @@
     </row>
     <row r="40" spans="1:7">
       <c r="A40">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B40" t="s">
         <v>38</v>
@@ -2869,7 +2869,7 @@
     </row>
     <row r="41" spans="1:7">
       <c r="A41">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B41" t="s">
         <v>38</v>
@@ -2892,7 +2892,7 @@
     </row>
     <row r="42" spans="1:7">
       <c r="A42">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B42" t="s">
         <v>39</v>
@@ -2915,7 +2915,7 @@
     </row>
     <row r="43" spans="1:7">
       <c r="A43">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B43" t="s">
         <v>40</v>
@@ -2938,7 +2938,7 @@
     </row>
     <row r="44" spans="1:7">
       <c r="A44">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B44" t="s">
         <v>40</v>
@@ -2961,7 +2961,7 @@
     </row>
     <row r="45" spans="1:7">
       <c r="A45">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B45" t="s">
         <v>40</v>
@@ -2984,7 +2984,7 @@
     </row>
     <row r="46" spans="1:7">
       <c r="A46">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B46" t="s">
         <v>41</v>
@@ -3007,7 +3007,7 @@
     </row>
     <row r="47" spans="1:7">
       <c r="A47">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B47" t="s">
         <v>42</v>
@@ -3030,7 +3030,7 @@
     </row>
     <row r="48" spans="1:7">
       <c r="A48">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B48" t="s">
         <v>43</v>
@@ -3053,7 +3053,7 @@
     </row>
     <row r="49" spans="1:7">
       <c r="A49">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B49" t="s">
         <v>44</v>
@@ -3076,7 +3076,7 @@
     </row>
     <row r="50" spans="1:7">
       <c r="A50">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B50" t="s">
         <v>45</v>
@@ -3099,7 +3099,7 @@
     </row>
     <row r="51" spans="1:7">
       <c r="A51">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B51" t="s">
         <v>45</v>
@@ -3122,7 +3122,7 @@
     </row>
     <row r="52" spans="1:7">
       <c r="A52">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B52" t="s">
         <v>46</v>
@@ -3145,7 +3145,7 @@
     </row>
     <row r="53" spans="1:7">
       <c r="A53">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B53" t="s">
         <v>47</v>
@@ -3168,7 +3168,7 @@
     </row>
     <row r="54" spans="1:7">
       <c r="A54">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B54" t="s">
         <v>47</v>
@@ -3191,7 +3191,7 @@
     </row>
     <row r="55" spans="1:7">
       <c r="A55">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B55" t="s">
         <v>48</v>
@@ -3214,7 +3214,7 @@
     </row>
     <row r="56" spans="1:7">
       <c r="A56">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B56" t="s">
         <v>49</v>
@@ -3237,7 +3237,7 @@
     </row>
     <row r="57" spans="1:7">
       <c r="A57">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B57" t="s">
         <v>50</v>
@@ -3260,7 +3260,7 @@
     </row>
     <row r="58" spans="1:7">
       <c r="A58">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B58" t="s">
         <v>50</v>
@@ -3283,7 +3283,7 @@
     </row>
     <row r="59" spans="1:7">
       <c r="A59">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B59" t="s">
         <v>51</v>
@@ -3306,7 +3306,7 @@
     </row>
     <row r="60" spans="1:7">
       <c r="A60">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B60" t="s">
         <v>52</v>
@@ -3329,7 +3329,7 @@
     </row>
     <row r="61" spans="1:7">
       <c r="A61">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B61" t="s">
         <v>52</v>
@@ -3352,7 +3352,7 @@
     </row>
     <row r="62" spans="1:7">
       <c r="A62">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B62" t="s">
         <v>53</v>
@@ -3375,7 +3375,7 @@
     </row>
     <row r="63" spans="1:7">
       <c r="A63">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B63" t="s">
         <v>54</v>
@@ -3398,7 +3398,7 @@
     </row>
     <row r="64" spans="1:7">
       <c r="A64">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B64" t="s">
         <v>55</v>
@@ -3421,7 +3421,7 @@
     </row>
     <row r="65" spans="1:7">
       <c r="A65">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B65" t="s">
         <v>55</v>
@@ -3444,7 +3444,7 @@
     </row>
     <row r="66" spans="1:7">
       <c r="A66">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B66" t="s">
         <v>56</v>
@@ -3467,7 +3467,7 @@
     </row>
     <row r="67" spans="1:7">
       <c r="A67">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B67" t="s">
         <v>57</v>
@@ -3490,7 +3490,7 @@
     </row>
     <row r="68" spans="1:7">
       <c r="A68">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B68" t="s">
         <v>58</v>
@@ -3513,7 +3513,7 @@
     </row>
     <row r="69" spans="1:7">
       <c r="A69">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B69" t="s">
         <v>58</v>
@@ -3536,7 +3536,7 @@
     </row>
     <row r="70" spans="1:7">
       <c r="A70">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B70" t="s">
         <v>58</v>
@@ -3559,7 +3559,7 @@
     </row>
     <row r="71" spans="1:7">
       <c r="A71">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B71" t="s">
         <v>59</v>
@@ -3582,7 +3582,7 @@
     </row>
     <row r="72" spans="1:7">
       <c r="A72">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B72" t="s">
         <v>60</v>
@@ -3605,7 +3605,7 @@
     </row>
     <row r="73" spans="1:7">
       <c r="A73">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B73" t="s">
         <v>61</v>
@@ -3628,7 +3628,7 @@
     </row>
     <row r="74" spans="1:7">
       <c r="A74">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B74" t="s">
         <v>61</v>
@@ -3651,7 +3651,7 @@
     </row>
     <row r="75" spans="1:7">
       <c r="A75">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B75" t="s">
         <v>62</v>
@@ -3674,7 +3674,7 @@
     </row>
     <row r="76" spans="1:7">
       <c r="A76">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B76" t="s">
         <v>62</v>
@@ -3697,7 +3697,7 @@
     </row>
     <row r="77" spans="1:7">
       <c r="A77">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B77" t="s">
         <v>62</v>
@@ -3720,7 +3720,7 @@
     </row>
     <row r="78" spans="1:7">
       <c r="A78">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B78" t="s">
         <v>63</v>
@@ -3743,7 +3743,7 @@
     </row>
     <row r="79" spans="1:7">
       <c r="A79">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B79" t="s">
         <v>63</v>
@@ -3766,7 +3766,7 @@
     </row>
     <row r="80" spans="1:7">
       <c r="A80">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B80" t="s">
         <v>64</v>
@@ -3789,7 +3789,7 @@
     </row>
     <row r="81" spans="1:7">
       <c r="A81">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B81" t="s">
         <v>65</v>
@@ -3812,7 +3812,7 @@
     </row>
     <row r="82" spans="1:7">
       <c r="A82">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B82" t="s">
         <v>66</v>
@@ -3835,7 +3835,7 @@
     </row>
     <row r="83" spans="1:7">
       <c r="A83">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B83" t="s">
         <v>67</v>
@@ -3858,7 +3858,7 @@
     </row>
     <row r="84" spans="1:7">
       <c r="A84">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B84" t="s">
         <v>68</v>
@@ -3881,7 +3881,7 @@
     </row>
     <row r="85" spans="1:7">
       <c r="A85">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B85" t="s">
         <v>69</v>
@@ -3904,7 +3904,7 @@
     </row>
     <row r="86" spans="1:7">
       <c r="A86">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B86" t="s">
         <v>70</v>
@@ -3927,7 +3927,7 @@
     </row>
     <row r="87" spans="1:7">
       <c r="A87">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B87" t="s">
         <v>70</v>
@@ -3950,7 +3950,7 @@
     </row>
     <row r="88" spans="1:7">
       <c r="A88">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B88" t="s">
         <v>71</v>
@@ -3973,7 +3973,7 @@
     </row>
     <row r="89" spans="1:7">
       <c r="A89">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B89" t="s">
         <v>71</v>
@@ -3996,7 +3996,7 @@
     </row>
     <row r="90" spans="1:7">
       <c r="A90">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B90" t="s">
         <v>72</v>
@@ -4019,7 +4019,7 @@
     </row>
     <row r="91" spans="1:7">
       <c r="A91">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B91" t="s">
         <v>73</v>
@@ -4042,7 +4042,7 @@
     </row>
     <row r="92" spans="1:7">
       <c r="A92">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B92" t="s">
         <v>73</v>
@@ -4065,7 +4065,7 @@
     </row>
     <row r="93" spans="1:7">
       <c r="A93">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B93" t="s">
         <v>74</v>
@@ -4088,7 +4088,7 @@
     </row>
     <row r="94" spans="1:7">
       <c r="A94">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B94" t="s">
         <v>75</v>
@@ -4111,7 +4111,7 @@
     </row>
     <row r="95" spans="1:7">
       <c r="A95">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B95" t="s">
         <v>76</v>
@@ -4134,7 +4134,7 @@
     </row>
     <row r="96" spans="1:7">
       <c r="A96">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B96" t="s">
         <v>77</v>
@@ -4157,7 +4157,7 @@
     </row>
     <row r="97" spans="1:7">
       <c r="A97">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B97" t="s">
         <v>78</v>
@@ -4180,7 +4180,7 @@
     </row>
     <row r="98" spans="1:7">
       <c r="A98">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B98" t="s">
         <v>79</v>
@@ -4203,7 +4203,7 @@
     </row>
     <row r="99" spans="1:7">
       <c r="A99">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B99" t="s">
         <v>80</v>
@@ -4226,7 +4226,7 @@
     </row>
     <row r="100" spans="1:7">
       <c r="A100">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B100" t="s">
         <v>81</v>
@@ -4249,7 +4249,7 @@
     </row>
     <row r="101" spans="1:7">
       <c r="A101">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B101" t="s">
         <v>82</v>
@@ -4272,7 +4272,7 @@
     </row>
     <row r="102" spans="1:7">
       <c r="A102">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B102" t="s">
         <v>83</v>
@@ -4295,7 +4295,7 @@
     </row>
     <row r="103" spans="1:7">
       <c r="A103">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B103" t="s">
         <v>84</v>
@@ -4318,7 +4318,7 @@
     </row>
     <row r="104" spans="1:7">
       <c r="A104">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B104" t="s">
         <v>85</v>
@@ -4341,7 +4341,7 @@
     </row>
     <row r="105" spans="1:7">
       <c r="A105">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B105" t="s">
         <v>85</v>
@@ -4364,7 +4364,7 @@
     </row>
     <row r="106" spans="1:7">
       <c r="A106">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B106" t="s">
         <v>86</v>
@@ -4387,7 +4387,7 @@
     </row>
     <row r="107" spans="1:7">
       <c r="A107">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B107" t="s">
         <v>87</v>
@@ -4410,7 +4410,7 @@
     </row>
     <row r="108" spans="1:7">
       <c r="A108">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B108" t="s">
         <v>87</v>
@@ -4433,7 +4433,7 @@
     </row>
     <row r="109" spans="1:7">
       <c r="A109">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B109" t="s">
         <v>88</v>
@@ -4456,7 +4456,7 @@
     </row>
     <row r="110" spans="1:7">
       <c r="A110">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B110" t="s">
         <v>88</v>
@@ -4479,7 +4479,7 @@
     </row>
     <row r="111" spans="1:7">
       <c r="A111">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B111" t="s">
         <v>89</v>
@@ -4502,7 +4502,7 @@
     </row>
     <row r="112" spans="1:7">
       <c r="A112">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B112" t="s">
         <v>89</v>
@@ -4525,7 +4525,7 @@
     </row>
     <row r="113" spans="1:7">
       <c r="A113">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B113" t="s">
         <v>90</v>
@@ -4548,7 +4548,7 @@
     </row>
     <row r="114" spans="1:7">
       <c r="A114">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B114" t="s">
         <v>90</v>
@@ -4571,7 +4571,7 @@
     </row>
     <row r="115" spans="1:7">
       <c r="A115">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B115" t="s">
         <v>91</v>
@@ -4594,7 +4594,7 @@
     </row>
     <row r="116" spans="1:7">
       <c r="A116">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B116" t="s">
         <v>92</v>
@@ -4617,7 +4617,7 @@
     </row>
     <row r="117" spans="1:7">
       <c r="A117">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B117" t="s">
         <v>93</v>
@@ -4640,7 +4640,7 @@
     </row>
     <row r="118" spans="1:7">
       <c r="A118">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B118" t="s">
         <v>94</v>
@@ -4663,7 +4663,7 @@
     </row>
     <row r="119" spans="1:7">
       <c r="A119">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B119" t="s">
         <v>95</v>
@@ -4686,7 +4686,7 @@
     </row>
     <row r="120" spans="1:7">
       <c r="A120">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B120" t="s">
         <v>96</v>
@@ -4709,7 +4709,7 @@
     </row>
     <row r="121" spans="1:7">
       <c r="A121">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B121" t="s">
         <v>97</v>
@@ -4732,7 +4732,7 @@
     </row>
     <row r="122" spans="1:7">
       <c r="A122">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B122" t="s">
         <v>98</v>
@@ -4755,7 +4755,7 @@
     </row>
     <row r="123" spans="1:7">
       <c r="A123">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B123" t="s">
         <v>99</v>
@@ -4778,7 +4778,7 @@
     </row>
     <row r="124" spans="1:7">
       <c r="A124">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B124" t="s">
         <v>100</v>
@@ -4801,7 +4801,7 @@
     </row>
     <row r="125" spans="1:7">
       <c r="A125">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B125" t="s">
         <v>101</v>
@@ -4824,7 +4824,7 @@
     </row>
     <row r="126" spans="1:7">
       <c r="A126">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B126" t="s">
         <v>102</v>
@@ -4847,7 +4847,7 @@
     </row>
     <row r="127" spans="1:7">
       <c r="A127">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B127" t="s">
         <v>103</v>
@@ -4870,7 +4870,7 @@
     </row>
     <row r="128" spans="1:7">
       <c r="A128">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B128" t="s">
         <v>104</v>
@@ -4893,7 +4893,7 @@
     </row>
     <row r="129" spans="1:7">
       <c r="A129">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B129" t="s">
         <v>105</v>
@@ -4916,7 +4916,7 @@
     </row>
     <row r="130" spans="1:7">
       <c r="A130">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B130" t="s">
         <v>105</v>
@@ -4939,7 +4939,7 @@
     </row>
     <row r="131" spans="1:7">
       <c r="A131">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B131" t="s">
         <v>106</v>
@@ -4962,7 +4962,7 @@
     </row>
     <row r="132" spans="1:7">
       <c r="A132">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B132" t="s">
         <v>107</v>
@@ -4985,7 +4985,7 @@
     </row>
     <row r="133" spans="1:7">
       <c r="A133">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B133" t="s">
         <v>108</v>
@@ -5008,7 +5008,7 @@
     </row>
     <row r="134" spans="1:7">
       <c r="A134">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B134" t="s">
         <v>108</v>
@@ -5031,7 +5031,7 @@
     </row>
     <row r="135" spans="1:7">
       <c r="A135">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B135" t="s">
         <v>109</v>
@@ -5054,7 +5054,7 @@
     </row>
     <row r="136" spans="1:7">
       <c r="A136">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B136" t="s">
         <v>110</v>
@@ -5077,7 +5077,7 @@
     </row>
     <row r="137" spans="1:7">
       <c r="A137">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B137" t="s">
         <v>111</v>
@@ -5100,7 +5100,7 @@
     </row>
     <row r="138" spans="1:7">
       <c r="A138">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B138" t="s">
         <v>112</v>
@@ -5123,7 +5123,7 @@
     </row>
     <row r="139" spans="1:7">
       <c r="A139">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B139" t="s">
         <v>113</v>
@@ -5146,7 +5146,7 @@
     </row>
     <row r="140" spans="1:7">
       <c r="A140">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B140" t="s">
         <v>114</v>
@@ -5169,7 +5169,7 @@
     </row>
     <row r="141" spans="1:7">
       <c r="A141">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B141" t="s">
         <v>115</v>
@@ -5192,7 +5192,7 @@
     </row>
     <row r="142" spans="1:7">
       <c r="A142">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B142" t="s">
         <v>116</v>
@@ -5215,7 +5215,7 @@
     </row>
     <row r="143" spans="1:7">
       <c r="A143">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B143" t="s">
         <v>117</v>
@@ -5238,7 +5238,7 @@
     </row>
     <row r="144" spans="1:7">
       <c r="A144">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B144" t="s">
         <v>117</v>
@@ -5261,7 +5261,7 @@
     </row>
     <row r="145" spans="1:7">
       <c r="A145">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B145" t="s">
         <v>118</v>
@@ -5284,7 +5284,7 @@
     </row>
     <row r="146" spans="1:7">
       <c r="A146">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B146" t="s">
         <v>119</v>
@@ -5307,7 +5307,7 @@
     </row>
     <row r="147" spans="1:7">
       <c r="A147">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B147" t="s">
         <v>120</v>
@@ -5330,7 +5330,7 @@
     </row>
     <row r="148" spans="1:7">
       <c r="A148">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B148" t="s">
         <v>120</v>
@@ -5353,7 +5353,7 @@
     </row>
     <row r="149" spans="1:7">
       <c r="A149">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B149" t="s">
         <v>121</v>
@@ -5376,7 +5376,7 @@
     </row>
     <row r="150" spans="1:7">
       <c r="A150">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B150" t="s">
         <v>121</v>
@@ -5399,7 +5399,7 @@
     </row>
     <row r="151" spans="1:7">
       <c r="A151">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B151" t="s">
         <v>122</v>
@@ -5422,7 +5422,7 @@
     </row>
     <row r="152" spans="1:7">
       <c r="A152">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B152" t="s">
         <v>123</v>
@@ -5445,7 +5445,7 @@
     </row>
     <row r="153" spans="1:7">
       <c r="A153">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B153" t="s">
         <v>124</v>
@@ -5468,7 +5468,7 @@
     </row>
     <row r="154" spans="1:7">
       <c r="A154">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B154" t="s">
         <v>124</v>
@@ -5491,7 +5491,7 @@
     </row>
     <row r="155" spans="1:7">
       <c r="A155">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B155" t="s">
         <v>125</v>
@@ -5514,7 +5514,7 @@
     </row>
     <row r="156" spans="1:7">
       <c r="A156">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B156" t="s">
         <v>126</v>
@@ -5537,7 +5537,7 @@
     </row>
     <row r="157" spans="1:7">
       <c r="A157">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B157" t="s">
         <v>127</v>
@@ -5560,7 +5560,7 @@
     </row>
     <row r="158" spans="1:7">
       <c r="A158">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B158" t="s">
         <v>128</v>
@@ -5583,7 +5583,7 @@
     </row>
     <row r="159" spans="1:7">
       <c r="A159">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B159" t="s">
         <v>129</v>
@@ -5606,7 +5606,7 @@
     </row>
     <row r="160" spans="1:7">
       <c r="A160">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B160" t="s">
         <v>130</v>
@@ -5629,7 +5629,7 @@
     </row>
     <row r="161" spans="1:7">
       <c r="A161">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B161" t="s">
         <v>131</v>
@@ -5652,7 +5652,7 @@
     </row>
     <row r="162" spans="1:7">
       <c r="A162">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B162" t="s">
         <v>132</v>
@@ -5675,7 +5675,7 @@
     </row>
     <row r="163" spans="1:7">
       <c r="A163">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B163" t="s">
         <v>133</v>
@@ -5698,7 +5698,7 @@
     </row>
     <row r="164" spans="1:7">
       <c r="A164">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B164" t="s">
         <v>134</v>
@@ -5721,7 +5721,7 @@
     </row>
     <row r="165" spans="1:7">
       <c r="A165">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B165" t="s">
         <v>135</v>
@@ -5744,7 +5744,7 @@
     </row>
     <row r="166" spans="1:7">
       <c r="A166">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B166" t="s">
         <v>136</v>
@@ -5767,7 +5767,7 @@
     </row>
     <row r="167" spans="1:7">
       <c r="A167">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B167" t="s">
         <v>136</v>
@@ -5790,7 +5790,7 @@
     </row>
     <row r="168" spans="1:7">
       <c r="A168">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B168" t="s">
         <v>137</v>
@@ -5813,7 +5813,7 @@
     </row>
     <row r="169" spans="1:7">
       <c r="A169">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B169" t="s">
         <v>138</v>
@@ -5836,7 +5836,7 @@
     </row>
     <row r="170" spans="1:7">
       <c r="A170">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B170" t="s">
         <v>139</v>
@@ -5859,7 +5859,7 @@
     </row>
     <row r="171" spans="1:7">
       <c r="A171">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B171" t="s">
         <v>140</v>
@@ -5882,7 +5882,7 @@
     </row>
     <row r="172" spans="1:7">
       <c r="A172">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B172" t="s">
         <v>141</v>
@@ -5905,7 +5905,7 @@
     </row>
     <row r="173" spans="1:7">
       <c r="A173">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B173" t="s">
         <v>142</v>
@@ -5928,7 +5928,7 @@
     </row>
     <row r="174" spans="1:7">
       <c r="A174">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B174" t="s">
         <v>143</v>
@@ -5951,7 +5951,7 @@
     </row>
     <row r="175" spans="1:7">
       <c r="A175">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B175" t="s">
         <v>144</v>
@@ -5974,7 +5974,7 @@
     </row>
     <row r="176" spans="1:7">
       <c r="A176">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B176" t="s">
         <v>145</v>
@@ -5997,7 +5997,7 @@
     </row>
     <row r="177" spans="1:7">
       <c r="A177">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B177" t="s">
         <v>146</v>
@@ -6020,7 +6020,7 @@
     </row>
     <row r="178" spans="1:7">
       <c r="A178">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B178" t="s">
         <v>147</v>
@@ -6043,7 +6043,7 @@
     </row>
     <row r="179" spans="1:7">
       <c r="A179">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B179" t="s">
         <v>148</v>
@@ -6066,7 +6066,7 @@
     </row>
     <row r="180" spans="1:7">
       <c r="A180">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B180" t="s">
         <v>149</v>
@@ -6089,7 +6089,7 @@
     </row>
     <row r="181" spans="1:7">
       <c r="A181">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B181" t="s">
         <v>150</v>
@@ -6112,7 +6112,7 @@
     </row>
     <row r="182" spans="1:7">
       <c r="A182">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B182" t="s">
         <v>151</v>
@@ -6135,7 +6135,7 @@
     </row>
     <row r="183" spans="1:7">
       <c r="A183">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B183" t="s">
         <v>152</v>
@@ -6158,7 +6158,7 @@
     </row>
     <row r="184" spans="1:7">
       <c r="A184">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B184" t="s">
         <v>153</v>
@@ -6181,7 +6181,7 @@
     </row>
     <row r="185" spans="1:7">
       <c r="A185">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B185" t="s">
         <v>154</v>
@@ -6204,7 +6204,7 @@
     </row>
     <row r="186" spans="1:7">
       <c r="A186">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B186" t="s">
         <v>155</v>
@@ -6227,7 +6227,7 @@
     </row>
     <row r="187" spans="1:7">
       <c r="A187">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B187" t="s">
         <v>156</v>
@@ -6250,7 +6250,7 @@
     </row>
     <row r="188" spans="1:7">
       <c r="A188">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B188" t="s">
         <v>156</v>
@@ -6273,7 +6273,7 @@
     </row>
     <row r="189" spans="1:7">
       <c r="A189">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B189" t="s">
         <v>156</v>
@@ -6296,7 +6296,7 @@
     </row>
     <row r="190" spans="1:7">
       <c r="A190">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B190" t="s">
         <v>157</v>
@@ -6319,7 +6319,7 @@
     </row>
     <row r="191" spans="1:7">
       <c r="A191">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B191" t="s">
         <v>157</v>
@@ -6342,7 +6342,7 @@
     </row>
     <row r="192" spans="1:7">
       <c r="A192">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B192" t="s">
         <v>158</v>
@@ -6365,7 +6365,7 @@
     </row>
     <row r="193" spans="1:7">
       <c r="A193">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B193" t="s">
         <v>159</v>
@@ -6388,7 +6388,7 @@
     </row>
     <row r="194" spans="1:7">
       <c r="A194">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B194" t="s">
         <v>160</v>
@@ -6411,7 +6411,7 @@
     </row>
     <row r="195" spans="1:7">
       <c r="A195">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B195" t="s">
         <v>161</v>
@@ -6434,7 +6434,7 @@
     </row>
     <row r="196" spans="1:7">
       <c r="A196">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B196" t="s">
         <v>162</v>
@@ -6457,7 +6457,7 @@
     </row>
     <row r="197" spans="1:7">
       <c r="A197">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B197" t="s">
         <v>163</v>
@@ -6480,7 +6480,7 @@
     </row>
     <row r="198" spans="1:7">
       <c r="A198">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B198" t="s">
         <v>163</v>
@@ -6503,7 +6503,7 @@
     </row>
     <row r="199" spans="1:7">
       <c r="A199">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B199" t="s">
         <v>164</v>
@@ -6526,7 +6526,7 @@
     </row>
     <row r="200" spans="1:7">
       <c r="A200">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B200" t="s">
         <v>165</v>
@@ -6549,7 +6549,7 @@
     </row>
     <row r="201" spans="1:7">
       <c r="A201">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B201" t="s">
         <v>166</v>
@@ -6572,7 +6572,7 @@
     </row>
     <row r="202" spans="1:7">
       <c r="A202">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B202" t="s">
         <v>167</v>
@@ -6595,7 +6595,7 @@
     </row>
     <row r="203" spans="1:7">
       <c r="A203">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B203" t="s">
         <v>168</v>
@@ -6618,7 +6618,7 @@
     </row>
     <row r="204" spans="1:7">
       <c r="A204">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B204" t="s">
         <v>169</v>
@@ -6641,7 +6641,7 @@
     </row>
     <row r="205" spans="1:7">
       <c r="A205">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B205" t="s">
         <v>169</v>
@@ -6664,7 +6664,7 @@
     </row>
     <row r="206" spans="1:7">
       <c r="A206">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B206" t="s">
         <v>170</v>
@@ -6687,7 +6687,7 @@
     </row>
     <row r="207" spans="1:7">
       <c r="A207">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B207" t="s">
         <v>171</v>
@@ -6710,7 +6710,7 @@
     </row>
     <row r="208" spans="1:7">
       <c r="A208">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B208" t="s">
         <v>172</v>
@@ -6733,7 +6733,7 @@
     </row>
     <row r="209" spans="1:7">
       <c r="A209">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B209" t="s">
         <v>173</v>
@@ -6756,7 +6756,7 @@
     </row>
     <row r="210" spans="1:7">
       <c r="A210">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B210" t="s">
         <v>174</v>
@@ -6779,7 +6779,7 @@
     </row>
     <row r="211" spans="1:7">
       <c r="A211">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B211" t="s">
         <v>175</v>
@@ -6802,7 +6802,7 @@
     </row>
     <row r="212" spans="1:7">
       <c r="A212">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B212" t="s">
         <v>176</v>
@@ -6825,7 +6825,7 @@
     </row>
     <row r="213" spans="1:7">
       <c r="A213">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B213" t="s">
         <v>177</v>
@@ -6848,7 +6848,7 @@
     </row>
     <row r="214" spans="1:7">
       <c r="A214">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B214" t="s">
         <v>178</v>
@@ -6871,7 +6871,7 @@
     </row>
     <row r="215" spans="1:7">
       <c r="A215">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B215" t="s">
         <v>179</v>
@@ -6894,7 +6894,7 @@
     </row>
     <row r="216" spans="1:7">
       <c r="A216">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B216" t="s">
         <v>179</v>
@@ -6917,7 +6917,7 @@
     </row>
     <row r="217" spans="1:7">
       <c r="A217">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B217" t="s">
         <v>180</v>
@@ -6940,7 +6940,7 @@
     </row>
     <row r="218" spans="1:7">
       <c r="A218">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B218" t="s">
         <v>181</v>
@@ -6963,7 +6963,7 @@
     </row>
     <row r="219" spans="1:7">
       <c r="A219">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B219" t="s">
         <v>181</v>
@@ -6986,7 +6986,7 @@
     </row>
     <row r="220" spans="1:7">
       <c r="A220">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B220" t="s">
         <v>182</v>
@@ -7009,7 +7009,7 @@
     </row>
     <row r="221" spans="1:7">
       <c r="A221">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B221" t="s">
         <v>182</v>
@@ -7032,7 +7032,7 @@
     </row>
     <row r="222" spans="1:7">
       <c r="A222">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B222" t="s">
         <v>183</v>
@@ -7055,7 +7055,7 @@
     </row>
     <row r="223" spans="1:7">
       <c r="A223">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B223" t="s">
         <v>184</v>
@@ -7078,7 +7078,7 @@
     </row>
     <row r="224" spans="1:7">
       <c r="A224">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B224" t="s">
         <v>185</v>
@@ -7101,7 +7101,7 @@
     </row>
     <row r="225" spans="1:7">
       <c r="A225">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B225" t="s">
         <v>186</v>
@@ -7124,7 +7124,7 @@
     </row>
     <row r="226" spans="1:7">
       <c r="A226">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B226" t="s">
         <v>187</v>
@@ -7147,7 +7147,7 @@
     </row>
     <row r="227" spans="1:7">
       <c r="A227">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B227" t="s">
         <v>187</v>
@@ -7170,7 +7170,7 @@
     </row>
     <row r="228" spans="1:7">
       <c r="A228">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B228" t="s">
         <v>188</v>
@@ -7193,7 +7193,7 @@
     </row>
     <row r="229" spans="1:7">
       <c r="A229">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B229" t="s">
         <v>188</v>
@@ -7216,7 +7216,7 @@
     </row>
     <row r="230" spans="1:7">
       <c r="A230">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B230" t="s">
         <v>189</v>
@@ -7239,7 +7239,7 @@
     </row>
     <row r="231" spans="1:7">
       <c r="A231">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B231" t="s">
         <v>190</v>
@@ -7262,7 +7262,7 @@
     </row>
     <row r="232" spans="1:7">
       <c r="A232">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B232" t="s">
         <v>190</v>
@@ -7285,7 +7285,7 @@
     </row>
     <row r="233" spans="1:7">
       <c r="A233">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B233" t="s">
         <v>191</v>
@@ -7308,7 +7308,7 @@
     </row>
     <row r="234" spans="1:7">
       <c r="A234">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B234" t="s">
         <v>192</v>
@@ -7331,7 +7331,7 @@
     </row>
     <row r="235" spans="1:7">
       <c r="A235">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B235" t="s">
         <v>193</v>
@@ -7354,7 +7354,7 @@
     </row>
     <row r="236" spans="1:7">
       <c r="A236">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B236" t="s">
         <v>194</v>
@@ -7377,7 +7377,7 @@
     </row>
     <row r="237" spans="1:7">
       <c r="A237">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B237" t="s">
         <v>194</v>
@@ -7400,7 +7400,7 @@
     </row>
     <row r="238" spans="1:7">
       <c r="A238">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B238" t="s">
         <v>195</v>
@@ -7423,7 +7423,7 @@
     </row>
     <row r="239" spans="1:7">
       <c r="A239">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B239" t="s">
         <v>195</v>
@@ -7446,7 +7446,7 @@
     </row>
     <row r="240" spans="1:7">
       <c r="A240">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B240" t="s">
         <v>195</v>
@@ -7469,7 +7469,7 @@
     </row>
     <row r="241" spans="1:7">
       <c r="A241">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B241" t="s">
         <v>196</v>
@@ -7492,7 +7492,7 @@
     </row>
     <row r="242" spans="1:7">
       <c r="A242">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B242" t="s">
         <v>196</v>
@@ -7515,7 +7515,7 @@
     </row>
     <row r="243" spans="1:7">
       <c r="A243">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B243" t="s">
         <v>197</v>
@@ -7538,7 +7538,7 @@
     </row>
     <row r="244" spans="1:7">
       <c r="A244">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B244" t="s">
         <v>197</v>
@@ -7585,7 +7585,7 @@
         <v>297</v>
       </c>
       <c r="B2">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -7593,7 +7593,7 @@
         <v>293</v>
       </c>
       <c r="B3">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -7665,7 +7665,7 @@
         <v>292</v>
       </c>
       <c r="B12">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -7697,7 +7697,7 @@
         <v>522</v>
       </c>
       <c r="B16">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>